<commit_message>
Added tables for market and payment elasticities
</commit_message>
<xml_diff>
--- a/Decoupling/Updates/tableTemplate.xlsx
+++ b/Decoupling/Updates/tableTemplate.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailmissouri-my.sharepoint.com/personal/ensxvd_umsystem_edu/Documents/FAPRI/MarketResearch/Decoupling/Updates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="114_{E64F9D53-B268-47B0-A535-E4631D69459A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2EBA5A18-8FA7-4374-A02D-2591256FCD55}"/>
+  <xr:revisionPtr revIDLastSave="150" documentId="114_{E64F9D53-B268-47B0-A535-E4631D69459A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{355A62F8-29B3-45EE-8BBC-8751F84D6D4A}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2C021E1E-A2C6-47E3-A832-2AA0528880E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="138">
   <si>
     <t>Other</t>
   </si>
@@ -321,6 +321,132 @@
   </si>
   <si>
     <t>PH</t>
+  </si>
+  <si>
+    <t>Elasticity: Market</t>
+  </si>
+  <si>
+    <t>Elasticity: Payment</t>
+  </si>
+  <si>
+    <t>EM_usNat1</t>
+  </si>
+  <si>
+    <t>EM_usNat2</t>
+  </si>
+  <si>
+    <t>EM_cornBelt1</t>
+  </si>
+  <si>
+    <t>EM_cornBelt2</t>
+  </si>
+  <si>
+    <t>EM_otherRegion1</t>
+  </si>
+  <si>
+    <t>EM_otherRegion2</t>
+  </si>
+  <si>
+    <t>EM_estPS1</t>
+  </si>
+  <si>
+    <t>EM_estPS2</t>
+  </si>
+  <si>
+    <t>EM_estMD1</t>
+  </si>
+  <si>
+    <t>EM_estMD2</t>
+  </si>
+  <si>
+    <t>EM_simuOrTheory1</t>
+  </si>
+  <si>
+    <t>EM_simuOrTheory2</t>
+  </si>
+  <si>
+    <t>EM_all1</t>
+  </si>
+  <si>
+    <t>EM_all2</t>
+  </si>
+  <si>
+    <t>EM_allCrossEffect1</t>
+  </si>
+  <si>
+    <t>EM_allCrossEffect2</t>
+  </si>
+  <si>
+    <t>EM_allCrops1</t>
+  </si>
+  <si>
+    <t>EM_allCrops2</t>
+  </si>
+  <si>
+    <t>EM_oneCrop1</t>
+  </si>
+  <si>
+    <t>EM_oneCrop2</t>
+  </si>
+  <si>
+    <t>EP_usNat1</t>
+  </si>
+  <si>
+    <t>EP_usNat2</t>
+  </si>
+  <si>
+    <t>EP_cornBelt1</t>
+  </si>
+  <si>
+    <t>EP_cornBelt2</t>
+  </si>
+  <si>
+    <t>EP_otherRegion1</t>
+  </si>
+  <si>
+    <t>EP_otherRegion2</t>
+  </si>
+  <si>
+    <t>EP_estPS1</t>
+  </si>
+  <si>
+    <t>EP_estPS2</t>
+  </si>
+  <si>
+    <t>EP_estMD1</t>
+  </si>
+  <si>
+    <t>EP_estMD2</t>
+  </si>
+  <si>
+    <t>EP_simuOrTheory1</t>
+  </si>
+  <si>
+    <t>EP_simuOrTheory2</t>
+  </si>
+  <si>
+    <t>EP_all1</t>
+  </si>
+  <si>
+    <t>EP_all2</t>
+  </si>
+  <si>
+    <t>EP_allCrossEffect1</t>
+  </si>
+  <si>
+    <t>EP_allCrossEffect2</t>
+  </si>
+  <si>
+    <t>EP_allCrops1</t>
+  </si>
+  <si>
+    <t>EP_allCrops2</t>
+  </si>
+  <si>
+    <t>EP_oneCrop1</t>
+  </si>
+  <si>
+    <t>EP_oneCrop2</t>
   </si>
 </sst>
 </file>
@@ -734,10 +860,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3CFEF19-65F2-4B7A-B20C-D8F1581CCEE7}">
-  <dimension ref="A1:V72"/>
+  <dimension ref="A1:V141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25:D26"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3676,6 +3802,2774 @@
     <row r="72" spans="1:22" x14ac:dyDescent="0.35">
       <c r="D72" s="7"/>
     </row>
+    <row r="73" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B73" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="2"/>
+    </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="C74" t="s">
+        <v>29</v>
+      </c>
+      <c r="E74" s="6"/>
+      <c r="G74" s="7"/>
+      <c r="J74" s="7"/>
+      <c r="M74" s="7"/>
+      <c r="P74" s="7"/>
+      <c r="S74" s="7"/>
+      <c r="V74" s="7"/>
+    </row>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>98</v>
+      </c>
+      <c r="D75" t="s">
+        <v>24</v>
+      </c>
+      <c r="E75" s="6">
+        <v>1</v>
+      </c>
+      <c r="F75" s="6">
+        <v>1</v>
+      </c>
+      <c r="G75" s="6">
+        <v>1</v>
+      </c>
+      <c r="H75" s="6">
+        <v>1</v>
+      </c>
+      <c r="I75" s="6">
+        <v>1</v>
+      </c>
+      <c r="J75" s="6">
+        <v>1</v>
+      </c>
+      <c r="K75" s="6">
+        <v>1</v>
+      </c>
+      <c r="L75" s="6">
+        <v>1</v>
+      </c>
+      <c r="M75" s="6">
+        <v>1</v>
+      </c>
+      <c r="N75" s="6">
+        <v>1</v>
+      </c>
+      <c r="O75" s="6">
+        <v>1</v>
+      </c>
+      <c r="P75" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q75" s="6">
+        <v>1</v>
+      </c>
+      <c r="R75" s="6">
+        <v>1</v>
+      </c>
+      <c r="S75" s="6">
+        <v>1</v>
+      </c>
+      <c r="T75" s="6">
+        <v>1</v>
+      </c>
+      <c r="U75" s="6">
+        <v>1</v>
+      </c>
+      <c r="V75" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>99</v>
+      </c>
+      <c r="D76" t="s">
+        <v>24</v>
+      </c>
+      <c r="E76" s="6">
+        <v>1</v>
+      </c>
+      <c r="F76" s="6">
+        <v>1</v>
+      </c>
+      <c r="G76" s="6">
+        <v>1</v>
+      </c>
+      <c r="H76" s="6">
+        <v>1</v>
+      </c>
+      <c r="I76" s="6">
+        <v>1</v>
+      </c>
+      <c r="J76" s="6">
+        <v>1</v>
+      </c>
+      <c r="K76" s="6">
+        <v>1</v>
+      </c>
+      <c r="L76" s="6">
+        <v>1</v>
+      </c>
+      <c r="M76" s="6">
+        <v>1</v>
+      </c>
+      <c r="N76" s="6">
+        <v>1</v>
+      </c>
+      <c r="O76" s="6">
+        <v>1</v>
+      </c>
+      <c r="P76" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q76" s="6">
+        <v>1</v>
+      </c>
+      <c r="R76" s="6">
+        <v>1</v>
+      </c>
+      <c r="S76" s="6">
+        <v>1</v>
+      </c>
+      <c r="T76" s="6">
+        <v>1</v>
+      </c>
+      <c r="U76" s="6">
+        <v>1</v>
+      </c>
+      <c r="V76" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="E77" s="6"/>
+      <c r="G77" s="7"/>
+      <c r="J77" s="7"/>
+      <c r="M77" s="7"/>
+      <c r="P77" s="7"/>
+      <c r="S77" s="7"/>
+      <c r="V77" s="7"/>
+    </row>
+    <row r="78" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>100</v>
+      </c>
+      <c r="D78" t="s">
+        <v>25</v>
+      </c>
+      <c r="E78" s="6">
+        <v>1</v>
+      </c>
+      <c r="F78" s="6">
+        <v>1</v>
+      </c>
+      <c r="G78" s="6">
+        <v>1</v>
+      </c>
+      <c r="H78" s="6">
+        <v>1</v>
+      </c>
+      <c r="I78" s="6">
+        <v>1</v>
+      </c>
+      <c r="J78" s="6">
+        <v>1</v>
+      </c>
+      <c r="K78" s="6">
+        <v>1</v>
+      </c>
+      <c r="L78" s="6">
+        <v>1</v>
+      </c>
+      <c r="M78" s="6">
+        <v>1</v>
+      </c>
+      <c r="N78" s="6">
+        <v>1</v>
+      </c>
+      <c r="O78" s="6">
+        <v>1</v>
+      </c>
+      <c r="P78" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q78" s="6">
+        <v>1</v>
+      </c>
+      <c r="R78" s="6">
+        <v>1</v>
+      </c>
+      <c r="S78" s="6">
+        <v>1</v>
+      </c>
+      <c r="T78" s="6">
+        <v>1</v>
+      </c>
+      <c r="U78" s="6">
+        <v>1</v>
+      </c>
+      <c r="V78" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>101</v>
+      </c>
+      <c r="D79" t="s">
+        <v>25</v>
+      </c>
+      <c r="E79" s="6">
+        <v>1</v>
+      </c>
+      <c r="F79" s="6">
+        <v>1</v>
+      </c>
+      <c r="G79" s="6">
+        <v>1</v>
+      </c>
+      <c r="H79" s="6">
+        <v>1</v>
+      </c>
+      <c r="I79" s="6">
+        <v>1</v>
+      </c>
+      <c r="J79" s="6">
+        <v>1</v>
+      </c>
+      <c r="K79" s="6">
+        <v>1</v>
+      </c>
+      <c r="L79" s="6">
+        <v>1</v>
+      </c>
+      <c r="M79" s="6">
+        <v>1</v>
+      </c>
+      <c r="N79" s="6">
+        <v>1</v>
+      </c>
+      <c r="O79" s="6">
+        <v>1</v>
+      </c>
+      <c r="P79" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q79" s="6">
+        <v>1</v>
+      </c>
+      <c r="R79" s="6">
+        <v>1</v>
+      </c>
+      <c r="S79" s="6">
+        <v>1</v>
+      </c>
+      <c r="T79" s="6">
+        <v>1</v>
+      </c>
+      <c r="U79" s="6">
+        <v>1</v>
+      </c>
+      <c r="V79" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="E80" s="6"/>
+      <c r="G80" s="7"/>
+      <c r="J80" s="7"/>
+      <c r="M80" s="7"/>
+      <c r="P80" s="7"/>
+      <c r="S80" s="7"/>
+      <c r="V80" s="7"/>
+    </row>
+    <row r="81" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>102</v>
+      </c>
+      <c r="D81" t="s">
+        <v>0</v>
+      </c>
+      <c r="E81" s="6">
+        <v>1</v>
+      </c>
+      <c r="F81" s="6">
+        <v>1</v>
+      </c>
+      <c r="G81" s="6">
+        <v>1</v>
+      </c>
+      <c r="H81" s="6">
+        <v>1</v>
+      </c>
+      <c r="I81" s="6">
+        <v>1</v>
+      </c>
+      <c r="J81" s="6">
+        <v>1</v>
+      </c>
+      <c r="K81" s="6">
+        <v>1</v>
+      </c>
+      <c r="L81" s="6">
+        <v>1</v>
+      </c>
+      <c r="M81" s="6">
+        <v>1</v>
+      </c>
+      <c r="N81" s="6">
+        <v>1</v>
+      </c>
+      <c r="O81" s="6">
+        <v>1</v>
+      </c>
+      <c r="P81" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q81" s="6">
+        <v>1</v>
+      </c>
+      <c r="R81" s="6">
+        <v>1</v>
+      </c>
+      <c r="S81" s="6">
+        <v>1</v>
+      </c>
+      <c r="T81" s="6">
+        <v>1</v>
+      </c>
+      <c r="U81" s="6">
+        <v>1</v>
+      </c>
+      <c r="V81" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>103</v>
+      </c>
+      <c r="D82" t="s">
+        <v>0</v>
+      </c>
+      <c r="E82" s="6">
+        <v>1</v>
+      </c>
+      <c r="F82" s="6">
+        <v>1</v>
+      </c>
+      <c r="G82" s="6">
+        <v>1</v>
+      </c>
+      <c r="H82" s="6">
+        <v>1</v>
+      </c>
+      <c r="I82" s="6">
+        <v>1</v>
+      </c>
+      <c r="J82" s="6">
+        <v>1</v>
+      </c>
+      <c r="K82" s="6">
+        <v>1</v>
+      </c>
+      <c r="L82" s="6">
+        <v>1</v>
+      </c>
+      <c r="M82" s="6">
+        <v>1</v>
+      </c>
+      <c r="N82" s="6">
+        <v>1</v>
+      </c>
+      <c r="O82" s="6">
+        <v>1</v>
+      </c>
+      <c r="P82" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q82" s="6">
+        <v>1</v>
+      </c>
+      <c r="R82" s="6">
+        <v>1</v>
+      </c>
+      <c r="S82" s="6">
+        <v>1</v>
+      </c>
+      <c r="T82" s="6">
+        <v>1</v>
+      </c>
+      <c r="U82" s="6">
+        <v>1</v>
+      </c>
+      <c r="V82" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="E83" s="6"/>
+      <c r="G83" s="7"/>
+      <c r="J83" s="7"/>
+      <c r="M83" s="7"/>
+      <c r="P83" s="7"/>
+      <c r="S83" s="7"/>
+      <c r="V83" s="7"/>
+    </row>
+    <row r="84" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="C84" t="s">
+        <v>28</v>
+      </c>
+      <c r="E84" s="6"/>
+      <c r="G84" s="7"/>
+      <c r="J84" s="7"/>
+      <c r="M84" s="7"/>
+      <c r="P84" s="7"/>
+      <c r="S84" s="7"/>
+      <c r="V84" s="7"/>
+    </row>
+    <row r="85" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>104</v>
+      </c>
+      <c r="D85" t="s">
+        <v>34</v>
+      </c>
+      <c r="E85" s="6">
+        <v>1</v>
+      </c>
+      <c r="F85" s="6">
+        <v>1</v>
+      </c>
+      <c r="G85" s="6">
+        <v>1</v>
+      </c>
+      <c r="H85" s="6">
+        <v>1</v>
+      </c>
+      <c r="I85" s="6">
+        <v>1</v>
+      </c>
+      <c r="J85" s="6">
+        <v>1</v>
+      </c>
+      <c r="K85" s="6">
+        <v>1</v>
+      </c>
+      <c r="L85" s="6">
+        <v>1</v>
+      </c>
+      <c r="M85" s="6">
+        <v>1</v>
+      </c>
+      <c r="N85" s="6">
+        <v>1</v>
+      </c>
+      <c r="O85" s="6">
+        <v>1</v>
+      </c>
+      <c r="P85" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q85" s="6">
+        <v>1</v>
+      </c>
+      <c r="R85" s="6">
+        <v>1</v>
+      </c>
+      <c r="S85" s="6">
+        <v>1</v>
+      </c>
+      <c r="T85" s="6">
+        <v>1</v>
+      </c>
+      <c r="U85" s="6">
+        <v>1</v>
+      </c>
+      <c r="V85" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>105</v>
+      </c>
+      <c r="D86" t="s">
+        <v>34</v>
+      </c>
+      <c r="E86" s="6">
+        <v>1</v>
+      </c>
+      <c r="F86" s="6">
+        <v>1</v>
+      </c>
+      <c r="G86" s="6">
+        <v>1</v>
+      </c>
+      <c r="H86" s="6">
+        <v>1</v>
+      </c>
+      <c r="I86" s="6">
+        <v>1</v>
+      </c>
+      <c r="J86" s="6">
+        <v>1</v>
+      </c>
+      <c r="K86" s="6">
+        <v>1</v>
+      </c>
+      <c r="L86" s="6">
+        <v>1</v>
+      </c>
+      <c r="M86" s="6">
+        <v>1</v>
+      </c>
+      <c r="N86" s="6">
+        <v>1</v>
+      </c>
+      <c r="O86" s="6">
+        <v>1</v>
+      </c>
+      <c r="P86" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q86" s="6">
+        <v>1</v>
+      </c>
+      <c r="R86" s="6">
+        <v>1</v>
+      </c>
+      <c r="S86" s="6">
+        <v>1</v>
+      </c>
+      <c r="T86" s="6">
+        <v>1</v>
+      </c>
+      <c r="U86" s="6">
+        <v>1</v>
+      </c>
+      <c r="V86" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="E87" s="6"/>
+      <c r="G87" s="7"/>
+      <c r="J87" s="7"/>
+      <c r="M87" s="7"/>
+      <c r="P87" s="7"/>
+      <c r="S87" s="7"/>
+      <c r="V87" s="7"/>
+    </row>
+    <row r="88" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>106</v>
+      </c>
+      <c r="D88" t="s">
+        <v>35</v>
+      </c>
+      <c r="E88" s="6">
+        <v>1</v>
+      </c>
+      <c r="F88" s="6">
+        <v>1</v>
+      </c>
+      <c r="G88" s="6">
+        <v>1</v>
+      </c>
+      <c r="H88" s="6">
+        <v>1</v>
+      </c>
+      <c r="I88" s="6">
+        <v>1</v>
+      </c>
+      <c r="J88" s="6">
+        <v>1</v>
+      </c>
+      <c r="K88" s="6">
+        <v>1</v>
+      </c>
+      <c r="L88" s="6">
+        <v>1</v>
+      </c>
+      <c r="M88" s="6">
+        <v>1</v>
+      </c>
+      <c r="N88" s="6">
+        <v>1</v>
+      </c>
+      <c r="O88" s="6">
+        <v>1</v>
+      </c>
+      <c r="P88" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q88" s="6">
+        <v>1</v>
+      </c>
+      <c r="R88" s="6">
+        <v>1</v>
+      </c>
+      <c r="S88" s="6">
+        <v>1</v>
+      </c>
+      <c r="T88" s="6">
+        <v>1</v>
+      </c>
+      <c r="U88" s="6">
+        <v>1</v>
+      </c>
+      <c r="V88" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>107</v>
+      </c>
+      <c r="D89" t="s">
+        <v>35</v>
+      </c>
+      <c r="E89" s="6">
+        <v>1</v>
+      </c>
+      <c r="F89" s="6">
+        <v>1</v>
+      </c>
+      <c r="G89" s="6">
+        <v>1</v>
+      </c>
+      <c r="H89" s="6">
+        <v>1</v>
+      </c>
+      <c r="I89" s="6">
+        <v>1</v>
+      </c>
+      <c r="J89" s="6">
+        <v>1</v>
+      </c>
+      <c r="K89" s="6">
+        <v>1</v>
+      </c>
+      <c r="L89" s="6">
+        <v>1</v>
+      </c>
+      <c r="M89" s="6">
+        <v>1</v>
+      </c>
+      <c r="N89" s="6">
+        <v>1</v>
+      </c>
+      <c r="O89" s="6">
+        <v>1</v>
+      </c>
+      <c r="P89" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q89" s="6">
+        <v>1</v>
+      </c>
+      <c r="R89" s="6">
+        <v>1</v>
+      </c>
+      <c r="S89" s="6">
+        <v>1</v>
+      </c>
+      <c r="T89" s="6">
+        <v>1</v>
+      </c>
+      <c r="U89" s="6">
+        <v>1</v>
+      </c>
+      <c r="V89" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="E90" s="6"/>
+      <c r="G90" s="7"/>
+      <c r="J90" s="7"/>
+      <c r="M90" s="7"/>
+      <c r="P90" s="7"/>
+      <c r="S90" s="7"/>
+      <c r="V90" s="7"/>
+    </row>
+    <row r="91" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>108</v>
+      </c>
+      <c r="D91" t="s">
+        <v>26</v>
+      </c>
+      <c r="E91" s="6">
+        <v>1</v>
+      </c>
+      <c r="F91" s="6">
+        <v>1</v>
+      </c>
+      <c r="G91" s="6">
+        <v>1</v>
+      </c>
+      <c r="H91" s="6">
+        <v>1</v>
+      </c>
+      <c r="I91" s="6">
+        <v>1</v>
+      </c>
+      <c r="J91" s="6">
+        <v>1</v>
+      </c>
+      <c r="K91" s="6">
+        <v>1</v>
+      </c>
+      <c r="L91" s="6">
+        <v>1</v>
+      </c>
+      <c r="M91" s="6">
+        <v>1</v>
+      </c>
+      <c r="N91" s="6">
+        <v>1</v>
+      </c>
+      <c r="O91" s="6">
+        <v>1</v>
+      </c>
+      <c r="P91" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q91" s="6">
+        <v>1</v>
+      </c>
+      <c r="R91" s="6">
+        <v>1</v>
+      </c>
+      <c r="S91" s="6">
+        <v>1</v>
+      </c>
+      <c r="T91" s="6">
+        <v>1</v>
+      </c>
+      <c r="U91" s="6">
+        <v>1</v>
+      </c>
+      <c r="V91" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>109</v>
+      </c>
+      <c r="D92" t="s">
+        <v>26</v>
+      </c>
+      <c r="E92" s="6">
+        <v>1</v>
+      </c>
+      <c r="F92" s="6">
+        <v>1</v>
+      </c>
+      <c r="G92" s="6">
+        <v>1</v>
+      </c>
+      <c r="H92" s="6">
+        <v>1</v>
+      </c>
+      <c r="I92" s="6">
+        <v>1</v>
+      </c>
+      <c r="J92" s="6">
+        <v>1</v>
+      </c>
+      <c r="K92" s="6">
+        <v>1</v>
+      </c>
+      <c r="L92" s="6">
+        <v>1</v>
+      </c>
+      <c r="M92" s="6">
+        <v>1</v>
+      </c>
+      <c r="N92" s="6">
+        <v>1</v>
+      </c>
+      <c r="O92" s="6">
+        <v>1</v>
+      </c>
+      <c r="P92" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q92" s="6">
+        <v>1</v>
+      </c>
+      <c r="R92" s="6">
+        <v>1</v>
+      </c>
+      <c r="S92" s="6">
+        <v>1</v>
+      </c>
+      <c r="T92" s="6">
+        <v>1</v>
+      </c>
+      <c r="U92" s="6">
+        <v>1</v>
+      </c>
+      <c r="V92" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="E93" s="6"/>
+      <c r="G93" s="7"/>
+      <c r="J93" s="7"/>
+      <c r="M93" s="7"/>
+      <c r="P93" s="7"/>
+      <c r="S93" s="7"/>
+      <c r="V93" s="7"/>
+    </row>
+    <row r="94" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="C94" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="95" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>110</v>
+      </c>
+      <c r="D95" t="s">
+        <v>27</v>
+      </c>
+      <c r="E95" s="6">
+        <v>1</v>
+      </c>
+      <c r="F95" s="6">
+        <v>1</v>
+      </c>
+      <c r="G95" s="6">
+        <v>1</v>
+      </c>
+      <c r="H95" s="6">
+        <v>1</v>
+      </c>
+      <c r="I95" s="6">
+        <v>1</v>
+      </c>
+      <c r="J95" s="6">
+        <v>1</v>
+      </c>
+      <c r="K95" s="6">
+        <v>1</v>
+      </c>
+      <c r="L95" s="6">
+        <v>1</v>
+      </c>
+      <c r="M95" s="6">
+        <v>1</v>
+      </c>
+      <c r="N95" s="6">
+        <v>1</v>
+      </c>
+      <c r="O95" s="6">
+        <v>1</v>
+      </c>
+      <c r="P95" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q95" s="6">
+        <v>1</v>
+      </c>
+      <c r="R95" s="6">
+        <v>1</v>
+      </c>
+      <c r="S95" s="6">
+        <v>1</v>
+      </c>
+      <c r="T95" s="6">
+        <v>1</v>
+      </c>
+      <c r="U95" s="6">
+        <v>1</v>
+      </c>
+      <c r="V95" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>111</v>
+      </c>
+      <c r="D96" t="s">
+        <v>27</v>
+      </c>
+      <c r="E96" s="6">
+        <v>1</v>
+      </c>
+      <c r="F96" s="6">
+        <v>1</v>
+      </c>
+      <c r="G96" s="6">
+        <v>1</v>
+      </c>
+      <c r="H96" s="6">
+        <v>1</v>
+      </c>
+      <c r="I96" s="6">
+        <v>1</v>
+      </c>
+      <c r="J96" s="6">
+        <v>1</v>
+      </c>
+      <c r="K96" s="6">
+        <v>1</v>
+      </c>
+      <c r="L96" s="6">
+        <v>1</v>
+      </c>
+      <c r="M96" s="6">
+        <v>1</v>
+      </c>
+      <c r="N96" s="6">
+        <v>1</v>
+      </c>
+      <c r="O96" s="6">
+        <v>1</v>
+      </c>
+      <c r="P96" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q96" s="6">
+        <v>1</v>
+      </c>
+      <c r="R96" s="6">
+        <v>1</v>
+      </c>
+      <c r="S96" s="6">
+        <v>1</v>
+      </c>
+      <c r="T96" s="6">
+        <v>1</v>
+      </c>
+      <c r="U96" s="6">
+        <v>1</v>
+      </c>
+      <c r="V96" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="E97" s="6"/>
+      <c r="F97" s="8"/>
+      <c r="G97" s="8"/>
+      <c r="H97" s="8"/>
+      <c r="I97" s="8"/>
+      <c r="J97" s="8"/>
+      <c r="K97" s="8"/>
+      <c r="L97" s="8"/>
+      <c r="M97" s="8"/>
+      <c r="N97" s="8"/>
+      <c r="O97" s="8"/>
+      <c r="P97" s="8"/>
+      <c r="Q97" s="8"/>
+      <c r="R97" s="8"/>
+      <c r="S97" s="8"/>
+      <c r="T97" s="8"/>
+      <c r="U97" s="8"/>
+      <c r="V97" s="8"/>
+    </row>
+    <row r="98" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="C98" t="s">
+        <v>30</v>
+      </c>
+      <c r="E98" s="6"/>
+      <c r="G98" s="7"/>
+      <c r="J98" s="7"/>
+      <c r="M98" s="7"/>
+      <c r="P98" s="7"/>
+      <c r="S98" s="7"/>
+      <c r="V98" s="7"/>
+    </row>
+    <row r="99" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>112</v>
+      </c>
+      <c r="D99" t="s">
+        <v>31</v>
+      </c>
+      <c r="E99" s="6">
+        <v>1</v>
+      </c>
+      <c r="F99" s="6">
+        <v>1</v>
+      </c>
+      <c r="G99" s="6">
+        <v>1</v>
+      </c>
+      <c r="H99" s="6">
+        <v>1</v>
+      </c>
+      <c r="I99" s="6">
+        <v>1</v>
+      </c>
+      <c r="J99" s="6">
+        <v>1</v>
+      </c>
+      <c r="K99" s="6">
+        <v>1</v>
+      </c>
+      <c r="L99" s="6">
+        <v>1</v>
+      </c>
+      <c r="M99" s="6">
+        <v>1</v>
+      </c>
+      <c r="N99" s="6">
+        <v>1</v>
+      </c>
+      <c r="O99" s="6">
+        <v>1</v>
+      </c>
+      <c r="P99" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q99" s="6">
+        <v>1</v>
+      </c>
+      <c r="R99" s="6">
+        <v>1</v>
+      </c>
+      <c r="S99" s="6">
+        <v>1</v>
+      </c>
+      <c r="T99" s="6">
+        <v>1</v>
+      </c>
+      <c r="U99" s="6">
+        <v>1</v>
+      </c>
+      <c r="V99" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>113</v>
+      </c>
+      <c r="D100" t="s">
+        <v>31</v>
+      </c>
+      <c r="E100" s="6">
+        <v>1</v>
+      </c>
+      <c r="F100" s="6">
+        <v>1</v>
+      </c>
+      <c r="G100" s="6">
+        <v>1</v>
+      </c>
+      <c r="H100" s="6">
+        <v>1</v>
+      </c>
+      <c r="I100" s="6">
+        <v>1</v>
+      </c>
+      <c r="J100" s="6">
+        <v>1</v>
+      </c>
+      <c r="K100" s="6">
+        <v>1</v>
+      </c>
+      <c r="L100" s="6">
+        <v>1</v>
+      </c>
+      <c r="M100" s="6">
+        <v>1</v>
+      </c>
+      <c r="N100" s="6">
+        <v>1</v>
+      </c>
+      <c r="O100" s="6">
+        <v>1</v>
+      </c>
+      <c r="P100" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q100" s="6">
+        <v>1</v>
+      </c>
+      <c r="R100" s="6">
+        <v>1</v>
+      </c>
+      <c r="S100" s="6">
+        <v>1</v>
+      </c>
+      <c r="T100" s="6">
+        <v>1</v>
+      </c>
+      <c r="U100" s="6">
+        <v>1</v>
+      </c>
+      <c r="V100" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="E101" s="6"/>
+      <c r="G101" s="7"/>
+      <c r="J101" s="7"/>
+      <c r="M101" s="7"/>
+      <c r="P101" s="7"/>
+      <c r="S101" s="7"/>
+      <c r="V101" s="7"/>
+    </row>
+    <row r="102" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>114</v>
+      </c>
+      <c r="D102" t="s">
+        <v>32</v>
+      </c>
+      <c r="E102" s="6">
+        <v>1</v>
+      </c>
+      <c r="F102" s="6">
+        <v>1</v>
+      </c>
+      <c r="G102" s="6">
+        <v>1</v>
+      </c>
+      <c r="H102" s="6">
+        <v>1</v>
+      </c>
+      <c r="I102" s="6">
+        <v>1</v>
+      </c>
+      <c r="J102" s="6">
+        <v>1</v>
+      </c>
+      <c r="K102" s="6">
+        <v>1</v>
+      </c>
+      <c r="L102" s="6">
+        <v>1</v>
+      </c>
+      <c r="M102" s="6">
+        <v>1</v>
+      </c>
+      <c r="N102" s="6">
+        <v>1</v>
+      </c>
+      <c r="O102" s="6">
+        <v>1</v>
+      </c>
+      <c r="P102" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q102" s="6">
+        <v>1</v>
+      </c>
+      <c r="R102" s="6">
+        <v>1</v>
+      </c>
+      <c r="S102" s="6">
+        <v>1</v>
+      </c>
+      <c r="T102" s="6">
+        <v>1</v>
+      </c>
+      <c r="U102" s="6">
+        <v>1</v>
+      </c>
+      <c r="V102" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>115</v>
+      </c>
+      <c r="D103" t="s">
+        <v>32</v>
+      </c>
+      <c r="E103" s="6">
+        <v>1</v>
+      </c>
+      <c r="F103" s="6">
+        <v>1</v>
+      </c>
+      <c r="G103" s="6">
+        <v>1</v>
+      </c>
+      <c r="H103" s="6">
+        <v>1</v>
+      </c>
+      <c r="I103" s="6">
+        <v>1</v>
+      </c>
+      <c r="J103" s="6">
+        <v>1</v>
+      </c>
+      <c r="K103" s="6">
+        <v>1</v>
+      </c>
+      <c r="L103" s="6">
+        <v>1</v>
+      </c>
+      <c r="M103" s="6">
+        <v>1</v>
+      </c>
+      <c r="N103" s="6">
+        <v>1</v>
+      </c>
+      <c r="O103" s="6">
+        <v>1</v>
+      </c>
+      <c r="P103" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q103" s="6">
+        <v>1</v>
+      </c>
+      <c r="R103" s="6">
+        <v>1</v>
+      </c>
+      <c r="S103" s="6">
+        <v>1</v>
+      </c>
+      <c r="T103" s="6">
+        <v>1</v>
+      </c>
+      <c r="U103" s="6">
+        <v>1</v>
+      </c>
+      <c r="V103" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="E104" s="6"/>
+      <c r="G104" s="7"/>
+      <c r="J104" s="7"/>
+      <c r="M104" s="7"/>
+      <c r="P104" s="7"/>
+      <c r="S104" s="7"/>
+      <c r="V104" s="7"/>
+    </row>
+    <row r="105" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>116</v>
+      </c>
+      <c r="D105" t="s">
+        <v>33</v>
+      </c>
+      <c r="E105" s="6">
+        <v>1</v>
+      </c>
+      <c r="F105" s="6">
+        <v>1</v>
+      </c>
+      <c r="G105" s="6">
+        <v>1</v>
+      </c>
+      <c r="H105" s="6">
+        <v>1</v>
+      </c>
+      <c r="I105" s="6">
+        <v>1</v>
+      </c>
+      <c r="J105" s="6">
+        <v>1</v>
+      </c>
+      <c r="K105" s="6">
+        <v>1</v>
+      </c>
+      <c r="L105" s="6">
+        <v>1</v>
+      </c>
+      <c r="M105" s="6">
+        <v>1</v>
+      </c>
+      <c r="N105" s="6">
+        <v>1</v>
+      </c>
+      <c r="O105" s="6">
+        <v>1</v>
+      </c>
+      <c r="P105" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q105" s="6">
+        <v>1</v>
+      </c>
+      <c r="R105" s="6">
+        <v>1</v>
+      </c>
+      <c r="S105" s="6">
+        <v>1</v>
+      </c>
+      <c r="T105" s="6">
+        <v>1</v>
+      </c>
+      <c r="U105" s="6">
+        <v>1</v>
+      </c>
+      <c r="V105" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>117</v>
+      </c>
+      <c r="D106" t="s">
+        <v>33</v>
+      </c>
+      <c r="E106" s="6">
+        <v>1</v>
+      </c>
+      <c r="F106" s="6">
+        <v>1</v>
+      </c>
+      <c r="G106" s="6">
+        <v>1</v>
+      </c>
+      <c r="H106" s="6">
+        <v>1</v>
+      </c>
+      <c r="I106" s="6">
+        <v>1</v>
+      </c>
+      <c r="J106" s="6">
+        <v>1</v>
+      </c>
+      <c r="K106" s="6">
+        <v>1</v>
+      </c>
+      <c r="L106" s="6">
+        <v>1</v>
+      </c>
+      <c r="M106" s="6">
+        <v>1</v>
+      </c>
+      <c r="N106" s="6">
+        <v>1</v>
+      </c>
+      <c r="O106" s="6">
+        <v>1</v>
+      </c>
+      <c r="P106" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q106" s="6">
+        <v>1</v>
+      </c>
+      <c r="R106" s="6">
+        <v>1</v>
+      </c>
+      <c r="S106" s="6">
+        <v>1</v>
+      </c>
+      <c r="T106" s="6">
+        <v>1</v>
+      </c>
+      <c r="U106" s="6">
+        <v>1</v>
+      </c>
+      <c r="V106" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B108" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C108" s="3"/>
+      <c r="D108" s="3"/>
+      <c r="E108" s="3"/>
+      <c r="F108" s="3"/>
+      <c r="G108" s="3"/>
+      <c r="H108" s="2"/>
+    </row>
+    <row r="109" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="C109" t="s">
+        <v>29</v>
+      </c>
+      <c r="E109" s="6"/>
+      <c r="G109" s="7"/>
+      <c r="J109" s="7"/>
+      <c r="M109" s="7"/>
+      <c r="P109" s="7"/>
+      <c r="S109" s="7"/>
+      <c r="V109" s="7"/>
+    </row>
+    <row r="110" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>118</v>
+      </c>
+      <c r="D110" t="s">
+        <v>24</v>
+      </c>
+      <c r="E110" s="6">
+        <v>1</v>
+      </c>
+      <c r="F110" s="6">
+        <v>1</v>
+      </c>
+      <c r="G110" s="6">
+        <v>1</v>
+      </c>
+      <c r="H110" s="6">
+        <v>1</v>
+      </c>
+      <c r="I110" s="6">
+        <v>1</v>
+      </c>
+      <c r="J110" s="6">
+        <v>1</v>
+      </c>
+      <c r="K110" s="6">
+        <v>1</v>
+      </c>
+      <c r="L110" s="6">
+        <v>1</v>
+      </c>
+      <c r="M110" s="6">
+        <v>1</v>
+      </c>
+      <c r="N110" s="6">
+        <v>1</v>
+      </c>
+      <c r="O110" s="6">
+        <v>1</v>
+      </c>
+      <c r="P110" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q110" s="6">
+        <v>1</v>
+      </c>
+      <c r="R110" s="6">
+        <v>1</v>
+      </c>
+      <c r="S110" s="6">
+        <v>1</v>
+      </c>
+      <c r="T110" s="6">
+        <v>1</v>
+      </c>
+      <c r="U110" s="6">
+        <v>1</v>
+      </c>
+      <c r="V110" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>119</v>
+      </c>
+      <c r="D111" t="s">
+        <v>24</v>
+      </c>
+      <c r="E111" s="6">
+        <v>1</v>
+      </c>
+      <c r="F111" s="6">
+        <v>1</v>
+      </c>
+      <c r="G111" s="6">
+        <v>1</v>
+      </c>
+      <c r="H111" s="6">
+        <v>1</v>
+      </c>
+      <c r="I111" s="6">
+        <v>1</v>
+      </c>
+      <c r="J111" s="6">
+        <v>1</v>
+      </c>
+      <c r="K111" s="6">
+        <v>1</v>
+      </c>
+      <c r="L111" s="6">
+        <v>1</v>
+      </c>
+      <c r="M111" s="6">
+        <v>1</v>
+      </c>
+      <c r="N111" s="6">
+        <v>1</v>
+      </c>
+      <c r="O111" s="6">
+        <v>1</v>
+      </c>
+      <c r="P111" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q111" s="6">
+        <v>1</v>
+      </c>
+      <c r="R111" s="6">
+        <v>1</v>
+      </c>
+      <c r="S111" s="6">
+        <v>1</v>
+      </c>
+      <c r="T111" s="6">
+        <v>1</v>
+      </c>
+      <c r="U111" s="6">
+        <v>1</v>
+      </c>
+      <c r="V111" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="E112" s="6"/>
+      <c r="G112" s="7"/>
+      <c r="J112" s="7"/>
+      <c r="M112" s="7"/>
+      <c r="P112" s="7"/>
+      <c r="S112" s="7"/>
+      <c r="V112" s="7"/>
+    </row>
+    <row r="113" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>120</v>
+      </c>
+      <c r="D113" t="s">
+        <v>25</v>
+      </c>
+      <c r="E113" s="6">
+        <v>1</v>
+      </c>
+      <c r="F113" s="6">
+        <v>1</v>
+      </c>
+      <c r="G113" s="6">
+        <v>1</v>
+      </c>
+      <c r="H113" s="6">
+        <v>1</v>
+      </c>
+      <c r="I113" s="6">
+        <v>1</v>
+      </c>
+      <c r="J113" s="6">
+        <v>1</v>
+      </c>
+      <c r="K113" s="6">
+        <v>1</v>
+      </c>
+      <c r="L113" s="6">
+        <v>1</v>
+      </c>
+      <c r="M113" s="6">
+        <v>1</v>
+      </c>
+      <c r="N113" s="6">
+        <v>1</v>
+      </c>
+      <c r="O113" s="6">
+        <v>1</v>
+      </c>
+      <c r="P113" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q113" s="6">
+        <v>1</v>
+      </c>
+      <c r="R113" s="6">
+        <v>1</v>
+      </c>
+      <c r="S113" s="6">
+        <v>1</v>
+      </c>
+      <c r="T113" s="6">
+        <v>1</v>
+      </c>
+      <c r="U113" s="6">
+        <v>1</v>
+      </c>
+      <c r="V113" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>121</v>
+      </c>
+      <c r="D114" t="s">
+        <v>25</v>
+      </c>
+      <c r="E114" s="6">
+        <v>1</v>
+      </c>
+      <c r="F114" s="6">
+        <v>1</v>
+      </c>
+      <c r="G114" s="6">
+        <v>1</v>
+      </c>
+      <c r="H114" s="6">
+        <v>1</v>
+      </c>
+      <c r="I114" s="6">
+        <v>1</v>
+      </c>
+      <c r="J114" s="6">
+        <v>1</v>
+      </c>
+      <c r="K114" s="6">
+        <v>1</v>
+      </c>
+      <c r="L114" s="6">
+        <v>1</v>
+      </c>
+      <c r="M114" s="6">
+        <v>1</v>
+      </c>
+      <c r="N114" s="6">
+        <v>1</v>
+      </c>
+      <c r="O114" s="6">
+        <v>1</v>
+      </c>
+      <c r="P114" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q114" s="6">
+        <v>1</v>
+      </c>
+      <c r="R114" s="6">
+        <v>1</v>
+      </c>
+      <c r="S114" s="6">
+        <v>1</v>
+      </c>
+      <c r="T114" s="6">
+        <v>1</v>
+      </c>
+      <c r="U114" s="6">
+        <v>1</v>
+      </c>
+      <c r="V114" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="E115" s="6"/>
+      <c r="G115" s="7"/>
+      <c r="J115" s="7"/>
+      <c r="M115" s="7"/>
+      <c r="P115" s="7"/>
+      <c r="S115" s="7"/>
+      <c r="V115" s="7"/>
+    </row>
+    <row r="116" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>122</v>
+      </c>
+      <c r="D116" t="s">
+        <v>0</v>
+      </c>
+      <c r="E116" s="6">
+        <v>1</v>
+      </c>
+      <c r="F116" s="6">
+        <v>1</v>
+      </c>
+      <c r="G116" s="6">
+        <v>1</v>
+      </c>
+      <c r="H116" s="6">
+        <v>1</v>
+      </c>
+      <c r="I116" s="6">
+        <v>1</v>
+      </c>
+      <c r="J116" s="6">
+        <v>1</v>
+      </c>
+      <c r="K116" s="6">
+        <v>1</v>
+      </c>
+      <c r="L116" s="6">
+        <v>1</v>
+      </c>
+      <c r="M116" s="6">
+        <v>1</v>
+      </c>
+      <c r="N116" s="6">
+        <v>1</v>
+      </c>
+      <c r="O116" s="6">
+        <v>1</v>
+      </c>
+      <c r="P116" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q116" s="6">
+        <v>1</v>
+      </c>
+      <c r="R116" s="6">
+        <v>1</v>
+      </c>
+      <c r="S116" s="6">
+        <v>1</v>
+      </c>
+      <c r="T116" s="6">
+        <v>1</v>
+      </c>
+      <c r="U116" s="6">
+        <v>1</v>
+      </c>
+      <c r="V116" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>123</v>
+      </c>
+      <c r="D117" t="s">
+        <v>0</v>
+      </c>
+      <c r="E117" s="6">
+        <v>1</v>
+      </c>
+      <c r="F117" s="6">
+        <v>1</v>
+      </c>
+      <c r="G117" s="6">
+        <v>1</v>
+      </c>
+      <c r="H117" s="6">
+        <v>1</v>
+      </c>
+      <c r="I117" s="6">
+        <v>1</v>
+      </c>
+      <c r="J117" s="6">
+        <v>1</v>
+      </c>
+      <c r="K117" s="6">
+        <v>1</v>
+      </c>
+      <c r="L117" s="6">
+        <v>1</v>
+      </c>
+      <c r="M117" s="6">
+        <v>1</v>
+      </c>
+      <c r="N117" s="6">
+        <v>1</v>
+      </c>
+      <c r="O117" s="6">
+        <v>1</v>
+      </c>
+      <c r="P117" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q117" s="6">
+        <v>1</v>
+      </c>
+      <c r="R117" s="6">
+        <v>1</v>
+      </c>
+      <c r="S117" s="6">
+        <v>1</v>
+      </c>
+      <c r="T117" s="6">
+        <v>1</v>
+      </c>
+      <c r="U117" s="6">
+        <v>1</v>
+      </c>
+      <c r="V117" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="E118" s="6"/>
+      <c r="G118" s="7"/>
+      <c r="J118" s="7"/>
+      <c r="M118" s="7"/>
+      <c r="P118" s="7"/>
+      <c r="S118" s="7"/>
+      <c r="V118" s="7"/>
+    </row>
+    <row r="119" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="C119" t="s">
+        <v>28</v>
+      </c>
+      <c r="E119" s="6"/>
+      <c r="G119" s="7"/>
+      <c r="J119" s="7"/>
+      <c r="M119" s="7"/>
+      <c r="P119" s="7"/>
+      <c r="S119" s="7"/>
+      <c r="V119" s="7"/>
+    </row>
+    <row r="120" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>124</v>
+      </c>
+      <c r="D120" t="s">
+        <v>34</v>
+      </c>
+      <c r="E120" s="6">
+        <v>1</v>
+      </c>
+      <c r="F120" s="6">
+        <v>1</v>
+      </c>
+      <c r="G120" s="6">
+        <v>1</v>
+      </c>
+      <c r="H120" s="6">
+        <v>1</v>
+      </c>
+      <c r="I120" s="6">
+        <v>1</v>
+      </c>
+      <c r="J120" s="6">
+        <v>1</v>
+      </c>
+      <c r="K120" s="6">
+        <v>1</v>
+      </c>
+      <c r="L120" s="6">
+        <v>1</v>
+      </c>
+      <c r="M120" s="6">
+        <v>1</v>
+      </c>
+      <c r="N120" s="6">
+        <v>1</v>
+      </c>
+      <c r="O120" s="6">
+        <v>1</v>
+      </c>
+      <c r="P120" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q120" s="6">
+        <v>1</v>
+      </c>
+      <c r="R120" s="6">
+        <v>1</v>
+      </c>
+      <c r="S120" s="6">
+        <v>1</v>
+      </c>
+      <c r="T120" s="6">
+        <v>1</v>
+      </c>
+      <c r="U120" s="6">
+        <v>1</v>
+      </c>
+      <c r="V120" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>125</v>
+      </c>
+      <c r="D121" t="s">
+        <v>34</v>
+      </c>
+      <c r="E121" s="6">
+        <v>1</v>
+      </c>
+      <c r="F121" s="6">
+        <v>1</v>
+      </c>
+      <c r="G121" s="6">
+        <v>1</v>
+      </c>
+      <c r="H121" s="6">
+        <v>1</v>
+      </c>
+      <c r="I121" s="6">
+        <v>1</v>
+      </c>
+      <c r="J121" s="6">
+        <v>1</v>
+      </c>
+      <c r="K121" s="6">
+        <v>1</v>
+      </c>
+      <c r="L121" s="6">
+        <v>1</v>
+      </c>
+      <c r="M121" s="6">
+        <v>1</v>
+      </c>
+      <c r="N121" s="6">
+        <v>1</v>
+      </c>
+      <c r="O121" s="6">
+        <v>1</v>
+      </c>
+      <c r="P121" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q121" s="6">
+        <v>1</v>
+      </c>
+      <c r="R121" s="6">
+        <v>1</v>
+      </c>
+      <c r="S121" s="6">
+        <v>1</v>
+      </c>
+      <c r="T121" s="6">
+        <v>1</v>
+      </c>
+      <c r="U121" s="6">
+        <v>1</v>
+      </c>
+      <c r="V121" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="E122" s="6"/>
+      <c r="G122" s="7"/>
+      <c r="J122" s="7"/>
+      <c r="M122" s="7"/>
+      <c r="P122" s="7"/>
+      <c r="S122" s="7"/>
+      <c r="V122" s="7"/>
+    </row>
+    <row r="123" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>126</v>
+      </c>
+      <c r="D123" t="s">
+        <v>35</v>
+      </c>
+      <c r="E123" s="6">
+        <v>1</v>
+      </c>
+      <c r="F123" s="6">
+        <v>1</v>
+      </c>
+      <c r="G123" s="6">
+        <v>1</v>
+      </c>
+      <c r="H123" s="6">
+        <v>1</v>
+      </c>
+      <c r="I123" s="6">
+        <v>1</v>
+      </c>
+      <c r="J123" s="6">
+        <v>1</v>
+      </c>
+      <c r="K123" s="6">
+        <v>1</v>
+      </c>
+      <c r="L123" s="6">
+        <v>1</v>
+      </c>
+      <c r="M123" s="6">
+        <v>1</v>
+      </c>
+      <c r="N123" s="6">
+        <v>1</v>
+      </c>
+      <c r="O123" s="6">
+        <v>1</v>
+      </c>
+      <c r="P123" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q123" s="6">
+        <v>1</v>
+      </c>
+      <c r="R123" s="6">
+        <v>1</v>
+      </c>
+      <c r="S123" s="6">
+        <v>1</v>
+      </c>
+      <c r="T123" s="6">
+        <v>1</v>
+      </c>
+      <c r="U123" s="6">
+        <v>1</v>
+      </c>
+      <c r="V123" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>127</v>
+      </c>
+      <c r="D124" t="s">
+        <v>35</v>
+      </c>
+      <c r="E124" s="6">
+        <v>1</v>
+      </c>
+      <c r="F124" s="6">
+        <v>1</v>
+      </c>
+      <c r="G124" s="6">
+        <v>1</v>
+      </c>
+      <c r="H124" s="6">
+        <v>1</v>
+      </c>
+      <c r="I124" s="6">
+        <v>1</v>
+      </c>
+      <c r="J124" s="6">
+        <v>1</v>
+      </c>
+      <c r="K124" s="6">
+        <v>1</v>
+      </c>
+      <c r="L124" s="6">
+        <v>1</v>
+      </c>
+      <c r="M124" s="6">
+        <v>1</v>
+      </c>
+      <c r="N124" s="6">
+        <v>1</v>
+      </c>
+      <c r="O124" s="6">
+        <v>1</v>
+      </c>
+      <c r="P124" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q124" s="6">
+        <v>1</v>
+      </c>
+      <c r="R124" s="6">
+        <v>1</v>
+      </c>
+      <c r="S124" s="6">
+        <v>1</v>
+      </c>
+      <c r="T124" s="6">
+        <v>1</v>
+      </c>
+      <c r="U124" s="6">
+        <v>1</v>
+      </c>
+      <c r="V124" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="E125" s="6"/>
+      <c r="G125" s="7"/>
+      <c r="J125" s="7"/>
+      <c r="M125" s="7"/>
+      <c r="P125" s="7"/>
+      <c r="S125" s="7"/>
+      <c r="V125" s="7"/>
+    </row>
+    <row r="126" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>128</v>
+      </c>
+      <c r="D126" t="s">
+        <v>26</v>
+      </c>
+      <c r="E126" s="6">
+        <v>1</v>
+      </c>
+      <c r="F126" s="6">
+        <v>1</v>
+      </c>
+      <c r="G126" s="6">
+        <v>1</v>
+      </c>
+      <c r="H126" s="6">
+        <v>1</v>
+      </c>
+      <c r="I126" s="6">
+        <v>1</v>
+      </c>
+      <c r="J126" s="6">
+        <v>1</v>
+      </c>
+      <c r="K126" s="6">
+        <v>1</v>
+      </c>
+      <c r="L126" s="6">
+        <v>1</v>
+      </c>
+      <c r="M126" s="6">
+        <v>1</v>
+      </c>
+      <c r="N126" s="6">
+        <v>1</v>
+      </c>
+      <c r="O126" s="6">
+        <v>1</v>
+      </c>
+      <c r="P126" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q126" s="6">
+        <v>1</v>
+      </c>
+      <c r="R126" s="6">
+        <v>1</v>
+      </c>
+      <c r="S126" s="6">
+        <v>1</v>
+      </c>
+      <c r="T126" s="6">
+        <v>1</v>
+      </c>
+      <c r="U126" s="6">
+        <v>1</v>
+      </c>
+      <c r="V126" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>129</v>
+      </c>
+      <c r="D127" t="s">
+        <v>26</v>
+      </c>
+      <c r="E127" s="6">
+        <v>1</v>
+      </c>
+      <c r="F127" s="6">
+        <v>1</v>
+      </c>
+      <c r="G127" s="6">
+        <v>1</v>
+      </c>
+      <c r="H127" s="6">
+        <v>1</v>
+      </c>
+      <c r="I127" s="6">
+        <v>1</v>
+      </c>
+      <c r="J127" s="6">
+        <v>1</v>
+      </c>
+      <c r="K127" s="6">
+        <v>1</v>
+      </c>
+      <c r="L127" s="6">
+        <v>1</v>
+      </c>
+      <c r="M127" s="6">
+        <v>1</v>
+      </c>
+      <c r="N127" s="6">
+        <v>1</v>
+      </c>
+      <c r="O127" s="6">
+        <v>1</v>
+      </c>
+      <c r="P127" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q127" s="6">
+        <v>1</v>
+      </c>
+      <c r="R127" s="6">
+        <v>1</v>
+      </c>
+      <c r="S127" s="6">
+        <v>1</v>
+      </c>
+      <c r="T127" s="6">
+        <v>1</v>
+      </c>
+      <c r="U127" s="6">
+        <v>1</v>
+      </c>
+      <c r="V127" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="E128" s="6"/>
+      <c r="G128" s="7"/>
+      <c r="J128" s="7"/>
+      <c r="M128" s="7"/>
+      <c r="P128" s="7"/>
+      <c r="S128" s="7"/>
+      <c r="V128" s="7"/>
+    </row>
+    <row r="129" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="C129" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="130" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>130</v>
+      </c>
+      <c r="D130" t="s">
+        <v>27</v>
+      </c>
+      <c r="E130" s="6">
+        <v>1</v>
+      </c>
+      <c r="F130" s="6">
+        <v>1</v>
+      </c>
+      <c r="G130" s="6">
+        <v>1</v>
+      </c>
+      <c r="H130" s="6">
+        <v>1</v>
+      </c>
+      <c r="I130" s="6">
+        <v>1</v>
+      </c>
+      <c r="J130" s="6">
+        <v>1</v>
+      </c>
+      <c r="K130" s="6">
+        <v>1</v>
+      </c>
+      <c r="L130" s="6">
+        <v>1</v>
+      </c>
+      <c r="M130" s="6">
+        <v>1</v>
+      </c>
+      <c r="N130" s="6">
+        <v>1</v>
+      </c>
+      <c r="O130" s="6">
+        <v>1</v>
+      </c>
+      <c r="P130" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q130" s="6">
+        <v>1</v>
+      </c>
+      <c r="R130" s="6">
+        <v>1</v>
+      </c>
+      <c r="S130" s="6">
+        <v>1</v>
+      </c>
+      <c r="T130" s="6">
+        <v>1</v>
+      </c>
+      <c r="U130" s="6">
+        <v>1</v>
+      </c>
+      <c r="V130" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>131</v>
+      </c>
+      <c r="D131" t="s">
+        <v>27</v>
+      </c>
+      <c r="E131" s="6">
+        <v>1</v>
+      </c>
+      <c r="F131" s="6">
+        <v>1</v>
+      </c>
+      <c r="G131" s="6">
+        <v>1</v>
+      </c>
+      <c r="H131" s="6">
+        <v>1</v>
+      </c>
+      <c r="I131" s="6">
+        <v>1</v>
+      </c>
+      <c r="J131" s="6">
+        <v>1</v>
+      </c>
+      <c r="K131" s="6">
+        <v>1</v>
+      </c>
+      <c r="L131" s="6">
+        <v>1</v>
+      </c>
+      <c r="M131" s="6">
+        <v>1</v>
+      </c>
+      <c r="N131" s="6">
+        <v>1</v>
+      </c>
+      <c r="O131" s="6">
+        <v>1</v>
+      </c>
+      <c r="P131" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q131" s="6">
+        <v>1</v>
+      </c>
+      <c r="R131" s="6">
+        <v>1</v>
+      </c>
+      <c r="S131" s="6">
+        <v>1</v>
+      </c>
+      <c r="T131" s="6">
+        <v>1</v>
+      </c>
+      <c r="U131" s="6">
+        <v>1</v>
+      </c>
+      <c r="V131" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="E132" s="6"/>
+      <c r="F132" s="8"/>
+      <c r="G132" s="8"/>
+      <c r="H132" s="8"/>
+      <c r="I132" s="8"/>
+      <c r="J132" s="8"/>
+      <c r="K132" s="8"/>
+      <c r="L132" s="8"/>
+      <c r="M132" s="8"/>
+      <c r="N132" s="8"/>
+      <c r="O132" s="8"/>
+      <c r="P132" s="8"/>
+      <c r="Q132" s="8"/>
+      <c r="R132" s="8"/>
+      <c r="S132" s="8"/>
+      <c r="T132" s="8"/>
+      <c r="U132" s="8"/>
+      <c r="V132" s="8"/>
+    </row>
+    <row r="133" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="C133" t="s">
+        <v>30</v>
+      </c>
+      <c r="E133" s="6"/>
+      <c r="G133" s="7"/>
+      <c r="J133" s="7"/>
+      <c r="M133" s="7"/>
+      <c r="P133" s="7"/>
+      <c r="S133" s="7"/>
+      <c r="V133" s="7"/>
+    </row>
+    <row r="134" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>132</v>
+      </c>
+      <c r="D134" t="s">
+        <v>31</v>
+      </c>
+      <c r="E134" s="6">
+        <v>1</v>
+      </c>
+      <c r="F134" s="6">
+        <v>1</v>
+      </c>
+      <c r="G134" s="6">
+        <v>1</v>
+      </c>
+      <c r="H134" s="6">
+        <v>1</v>
+      </c>
+      <c r="I134" s="6">
+        <v>1</v>
+      </c>
+      <c r="J134" s="6">
+        <v>1</v>
+      </c>
+      <c r="K134" s="6">
+        <v>1</v>
+      </c>
+      <c r="L134" s="6">
+        <v>1</v>
+      </c>
+      <c r="M134" s="6">
+        <v>1</v>
+      </c>
+      <c r="N134" s="6">
+        <v>1</v>
+      </c>
+      <c r="O134" s="6">
+        <v>1</v>
+      </c>
+      <c r="P134" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q134" s="6">
+        <v>1</v>
+      </c>
+      <c r="R134" s="6">
+        <v>1</v>
+      </c>
+      <c r="S134" s="6">
+        <v>1</v>
+      </c>
+      <c r="T134" s="6">
+        <v>1</v>
+      </c>
+      <c r="U134" s="6">
+        <v>1</v>
+      </c>
+      <c r="V134" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>133</v>
+      </c>
+      <c r="D135" t="s">
+        <v>31</v>
+      </c>
+      <c r="E135" s="6">
+        <v>1</v>
+      </c>
+      <c r="F135" s="6">
+        <v>1</v>
+      </c>
+      <c r="G135" s="6">
+        <v>1</v>
+      </c>
+      <c r="H135" s="6">
+        <v>1</v>
+      </c>
+      <c r="I135" s="6">
+        <v>1</v>
+      </c>
+      <c r="J135" s="6">
+        <v>1</v>
+      </c>
+      <c r="K135" s="6">
+        <v>1</v>
+      </c>
+      <c r="L135" s="6">
+        <v>1</v>
+      </c>
+      <c r="M135" s="6">
+        <v>1</v>
+      </c>
+      <c r="N135" s="6">
+        <v>1</v>
+      </c>
+      <c r="O135" s="6">
+        <v>1</v>
+      </c>
+      <c r="P135" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q135" s="6">
+        <v>1</v>
+      </c>
+      <c r="R135" s="6">
+        <v>1</v>
+      </c>
+      <c r="S135" s="6">
+        <v>1</v>
+      </c>
+      <c r="T135" s="6">
+        <v>1</v>
+      </c>
+      <c r="U135" s="6">
+        <v>1</v>
+      </c>
+      <c r="V135" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="E136" s="6"/>
+      <c r="G136" s="7"/>
+      <c r="J136" s="7"/>
+      <c r="M136" s="7"/>
+      <c r="P136" s="7"/>
+      <c r="S136" s="7"/>
+      <c r="V136" s="7"/>
+    </row>
+    <row r="137" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>134</v>
+      </c>
+      <c r="D137" t="s">
+        <v>32</v>
+      </c>
+      <c r="E137" s="6">
+        <v>1</v>
+      </c>
+      <c r="F137" s="6">
+        <v>1</v>
+      </c>
+      <c r="G137" s="6">
+        <v>1</v>
+      </c>
+      <c r="H137" s="6">
+        <v>1</v>
+      </c>
+      <c r="I137" s="6">
+        <v>1</v>
+      </c>
+      <c r="J137" s="6">
+        <v>1</v>
+      </c>
+      <c r="K137" s="6">
+        <v>1</v>
+      </c>
+      <c r="L137" s="6">
+        <v>1</v>
+      </c>
+      <c r="M137" s="6">
+        <v>1</v>
+      </c>
+      <c r="N137" s="6">
+        <v>1</v>
+      </c>
+      <c r="O137" s="6">
+        <v>1</v>
+      </c>
+      <c r="P137" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q137" s="6">
+        <v>1</v>
+      </c>
+      <c r="R137" s="6">
+        <v>1</v>
+      </c>
+      <c r="S137" s="6">
+        <v>1</v>
+      </c>
+      <c r="T137" s="6">
+        <v>1</v>
+      </c>
+      <c r="U137" s="6">
+        <v>1</v>
+      </c>
+      <c r="V137" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>135</v>
+      </c>
+      <c r="D138" t="s">
+        <v>32</v>
+      </c>
+      <c r="E138" s="6">
+        <v>1</v>
+      </c>
+      <c r="F138" s="6">
+        <v>1</v>
+      </c>
+      <c r="G138" s="6">
+        <v>1</v>
+      </c>
+      <c r="H138" s="6">
+        <v>1</v>
+      </c>
+      <c r="I138" s="6">
+        <v>1</v>
+      </c>
+      <c r="J138" s="6">
+        <v>1</v>
+      </c>
+      <c r="K138" s="6">
+        <v>1</v>
+      </c>
+      <c r="L138" s="6">
+        <v>1</v>
+      </c>
+      <c r="M138" s="6">
+        <v>1</v>
+      </c>
+      <c r="N138" s="6">
+        <v>1</v>
+      </c>
+      <c r="O138" s="6">
+        <v>1</v>
+      </c>
+      <c r="P138" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q138" s="6">
+        <v>1</v>
+      </c>
+      <c r="R138" s="6">
+        <v>1</v>
+      </c>
+      <c r="S138" s="6">
+        <v>1</v>
+      </c>
+      <c r="T138" s="6">
+        <v>1</v>
+      </c>
+      <c r="U138" s="6">
+        <v>1</v>
+      </c>
+      <c r="V138" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="E139" s="6"/>
+      <c r="G139" s="7"/>
+      <c r="J139" s="7"/>
+      <c r="M139" s="7"/>
+      <c r="P139" s="7"/>
+      <c r="S139" s="7"/>
+      <c r="V139" s="7"/>
+    </row>
+    <row r="140" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>136</v>
+      </c>
+      <c r="D140" t="s">
+        <v>33</v>
+      </c>
+      <c r="E140" s="6">
+        <v>1</v>
+      </c>
+      <c r="F140" s="6">
+        <v>1</v>
+      </c>
+      <c r="G140" s="6">
+        <v>1</v>
+      </c>
+      <c r="H140" s="6">
+        <v>1</v>
+      </c>
+      <c r="I140" s="6">
+        <v>1</v>
+      </c>
+      <c r="J140" s="6">
+        <v>1</v>
+      </c>
+      <c r="K140" s="6">
+        <v>1</v>
+      </c>
+      <c r="L140" s="6">
+        <v>1</v>
+      </c>
+      <c r="M140" s="6">
+        <v>1</v>
+      </c>
+      <c r="N140" s="6">
+        <v>1</v>
+      </c>
+      <c r="O140" s="6">
+        <v>1</v>
+      </c>
+      <c r="P140" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q140" s="6">
+        <v>1</v>
+      </c>
+      <c r="R140" s="6">
+        <v>1</v>
+      </c>
+      <c r="S140" s="6">
+        <v>1</v>
+      </c>
+      <c r="T140" s="6">
+        <v>1</v>
+      </c>
+      <c r="U140" s="6">
+        <v>1</v>
+      </c>
+      <c r="V140" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>137</v>
+      </c>
+      <c r="D141" t="s">
+        <v>33</v>
+      </c>
+      <c r="E141" s="6">
+        <v>1</v>
+      </c>
+      <c r="F141" s="6">
+        <v>1</v>
+      </c>
+      <c r="G141" s="6">
+        <v>1</v>
+      </c>
+      <c r="H141" s="6">
+        <v>1</v>
+      </c>
+      <c r="I141" s="6">
+        <v>1</v>
+      </c>
+      <c r="J141" s="6">
+        <v>1</v>
+      </c>
+      <c r="K141" s="6">
+        <v>1</v>
+      </c>
+      <c r="L141" s="6">
+        <v>1</v>
+      </c>
+      <c r="M141" s="6">
+        <v>1</v>
+      </c>
+      <c r="N141" s="6">
+        <v>1</v>
+      </c>
+      <c r="O141" s="6">
+        <v>1</v>
+      </c>
+      <c r="P141" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q141" s="6">
+        <v>1</v>
+      </c>
+      <c r="R141" s="6">
+        <v>1</v>
+      </c>
+      <c r="S141" s="6">
+        <v>1</v>
+      </c>
+      <c r="T141" s="6">
+        <v>1</v>
+      </c>
+      <c r="U141" s="6">
+        <v>1</v>
+      </c>
+      <c r="V141" s="6">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3683,21 +6577,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009AA21861009F844A94D45FCCECE366B4" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e658606205e1dbc8e3f5b77287602906">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c03d4cec-2a4e-42ae-b684-cd712438aa88" xmlns:ns4="8e23d785-2c7b-4ebd-b19b-adb2653ad200" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e7ada76741c526a1ec7a93ee9c23d7ee" ns3:_="" ns4:_="">
     <xsd:import namespace="c03d4cec-2a4e-42ae-b684-cd712438aa88"/>
@@ -3920,24 +6799,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE61CEFA-3C51-4AC5-B679-3D7FA08B806C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18DBFE82-80C8-4376-B234-6C09CB739632}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69518AF9-9CB4-408D-86CF-D237C82EA94C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3954,4 +6831,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18DBFE82-80C8-4376-B234-6C09CB739632}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE61CEFA-3C51-4AC5-B679-3D7FA08B806C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>